<commit_message>
Finish initial component placement
Need to route tracks next.
</commit_message>
<xml_diff>
--- a/Resources/00_Resource_Directory.xlsx
+++ b/Resources/00_Resource_Directory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\OneDrive\Desktop\60W-20V-Buck-Converter-in-CCM\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3B8A17-5F0B-4522-82DD-0D32599309F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{423EBA0F-86CF-4B98-B01D-8C8022D455D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>DOC#</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>App note shwing how to pick the value for cin (ceramic and elec) and cout.</t>
+  </si>
+  <si>
+    <t>App note shows vout ripple approximation - simulated on ltspice and is very close.</t>
   </si>
 </sst>
 </file>
@@ -408,7 +411,7 @@
   <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,8 +469,12 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>

</xml_diff>